<commit_message>
Added new SAS file, recreating table 14.2
</commit_message>
<xml_diff>
--- a/metadata/specs.xlsx
+++ b/metadata/specs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucfi\Documents\Clinical Data\ClinicalExercise\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF1980C-6DC5-4967-9B55-9CE213953C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E58A0E5-EDE3-484A-AFA2-1D04F35782E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -10032,9 +10032,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I996"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:G7"/>
+      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -11259,9 +11259,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S831"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C279" sqref="C279"/>
+      <selection pane="bottomLeft" activeCell="D245" sqref="D245:F246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -35580,9 +35580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H790"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A207" sqref="A207"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D230" sqref="D230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>